<commit_message>
Added Results for small Ts.
</commit_message>
<xml_diff>
--- a/Test Results/ResultsOnSlowPC.xlsx
+++ b/Test Results/ResultsOnSlowPC.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -170,15 +170,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -187,22 +184,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -223,6 +226,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -271,7 +277,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -306,7 +312,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -515,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T25"/>
+  <dimension ref="A1:X27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="S16" sqref="S16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,65 +552,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="I1" s="2" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="I1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2" t="s">
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="I2" s="2" t="s">
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="I2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2" t="s">
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2" t="s">
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2" t="s">
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
+      <c r="S2" s="12"/>
+      <c r="T2" s="12"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -666,7 +672,7 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="A4" s="12">
         <v>64</v>
       </c>
       <c r="B4" s="1">
@@ -728,7 +734,7 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="1">
         <v>489</v>
       </c>
@@ -788,7 +794,7 @@
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="A6" s="12"/>
       <c r="B6" s="1">
         <v>585</v>
       </c>
@@ -848,7 +854,7 @@
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="A7" s="12">
         <v>128</v>
       </c>
       <c r="B7" s="1">
@@ -910,7 +916,7 @@
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="12"/>
       <c r="B8" s="1">
         <v>673</v>
       </c>
@@ -970,7 +976,7 @@
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="1">
         <v>827</v>
       </c>
@@ -1030,701 +1036,868 @@
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="A10" s="13">
         <v>1024</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>2395</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>3247</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>691</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>34657</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <v>37932</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <v>10673</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="3">
         <v>29</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10" s="3">
         <v>317</v>
       </c>
-      <c r="K10" s="4">
+      <c r="K10" s="3">
         <v>352</v>
       </c>
-      <c r="L10" s="4">
+      <c r="L10" s="3">
         <v>356</v>
       </c>
-      <c r="M10" s="4">
+      <c r="M10" s="3">
         <v>3776</v>
       </c>
-      <c r="N10" s="4">
+      <c r="N10" s="3">
         <v>4135</v>
       </c>
-      <c r="O10" s="4">
+      <c r="O10" s="3">
         <v>28</v>
       </c>
-      <c r="P10" s="4">
+      <c r="P10" s="3">
         <v>330</v>
       </c>
-      <c r="Q10" s="4">
+      <c r="Q10" s="3">
         <v>352</v>
       </c>
-      <c r="R10" s="4">
+      <c r="R10" s="3">
         <v>352</v>
       </c>
-      <c r="S10" s="4">
+      <c r="S10" s="3">
         <v>3800</v>
       </c>
-      <c r="T10" s="5">
+      <c r="T10" s="4">
         <v>4130</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7">
+      <c r="A11" s="14"/>
+      <c r="B11" s="5">
         <v>3946</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="5">
         <v>1188</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="5">
         <v>636</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="5">
         <v>42680</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="5">
         <v>17110</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="5">
         <v>10020</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="H11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11" s="5">
         <v>2912</v>
       </c>
-      <c r="J11" s="7">
+      <c r="J11" s="5">
         <v>515</v>
       </c>
-      <c r="K11" s="7">
+      <c r="K11" s="5">
         <v>215</v>
       </c>
-      <c r="L11" s="7">
+      <c r="L11" s="5">
         <v>30355</v>
       </c>
-      <c r="M11" s="7">
+      <c r="M11" s="5">
         <v>5654</v>
       </c>
-      <c r="N11" s="7">
+      <c r="N11" s="5">
         <v>2459</v>
       </c>
-      <c r="O11" s="7">
+      <c r="O11" s="5">
         <v>2898</v>
       </c>
-      <c r="P11" s="7">
+      <c r="P11" s="5">
         <v>513</v>
       </c>
-      <c r="Q11" s="7">
+      <c r="Q11" s="5">
         <v>213</v>
       </c>
-      <c r="R11" s="7">
+      <c r="R11" s="5">
         <v>30461</v>
       </c>
-      <c r="S11" s="7">
+      <c r="S11" s="5">
         <v>5659</v>
       </c>
-      <c r="T11" s="8">
+      <c r="T11" s="6">
         <v>2442</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="7">
+      <c r="A12" s="14"/>
+      <c r="B12" s="5">
         <v>4319</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="5">
         <v>3235</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="5">
         <v>297</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="5">
         <v>53948</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="5">
         <v>38082</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="5">
         <v>3649</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="H12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I12" s="5">
         <v>4019</v>
       </c>
-      <c r="J12" s="7">
+      <c r="J12" s="5">
         <v>309</v>
       </c>
-      <c r="K12" s="7">
+      <c r="K12" s="5">
         <v>87</v>
       </c>
-      <c r="L12" s="7">
+      <c r="L12" s="5">
         <v>41031</v>
       </c>
-      <c r="M12" s="7">
+      <c r="M12" s="5">
         <v>4058</v>
       </c>
-      <c r="N12" s="7">
+      <c r="N12" s="5">
         <v>903</v>
       </c>
-      <c r="O12" s="7">
+      <c r="O12" s="5">
         <v>3977</v>
       </c>
-      <c r="P12" s="7">
+      <c r="P12" s="5">
         <v>311</v>
       </c>
-      <c r="Q12" s="7">
+      <c r="Q12" s="5">
         <v>87</v>
       </c>
-      <c r="R12" s="7">
+      <c r="R12" s="5">
         <v>39895</v>
       </c>
-      <c r="S12" s="7">
+      <c r="S12" s="5">
         <v>4044</v>
       </c>
-      <c r="T12" s="8">
+      <c r="T12" s="6">
         <v>887</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
+      <c r="A13" s="14">
         <v>2048</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="5">
         <v>4183</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="5">
         <v>5472</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="5">
         <v>700</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="5">
         <v>58783</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="5">
         <v>60580</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="5">
         <v>10630</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="H13" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I13" s="7">
+      <c r="I13" s="5">
         <v>28</v>
       </c>
-      <c r="J13" s="7">
+      <c r="J13" s="5">
         <v>330</v>
       </c>
-      <c r="K13" s="7">
+      <c r="K13" s="5">
         <v>355</v>
       </c>
-      <c r="L13" s="7">
+      <c r="L13" s="5">
         <v>304</v>
       </c>
-      <c r="M13" s="7">
+      <c r="M13" s="5">
         <v>3708</v>
       </c>
-      <c r="N13" s="7">
+      <c r="N13" s="5">
         <v>4136</v>
       </c>
-      <c r="O13" s="7">
+      <c r="O13" s="5">
         <v>29</v>
       </c>
-      <c r="P13" s="7">
+      <c r="P13" s="5">
         <v>329</v>
       </c>
-      <c r="Q13" s="7">
+      <c r="Q13" s="5">
         <v>352</v>
       </c>
-      <c r="R13" s="7">
+      <c r="R13" s="5">
         <v>317</v>
       </c>
-      <c r="S13" s="7">
+      <c r="S13" s="5">
         <v>3689</v>
       </c>
-      <c r="T13" s="8">
+      <c r="T13" s="6">
         <v>4122</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="7">
+      <c r="A14" s="14"/>
+      <c r="B14" s="5">
         <v>7398</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="5">
         <v>1217</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="5">
         <v>629</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="5">
         <v>68778</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="5">
         <v>17118</v>
       </c>
-      <c r="G14" s="7">
+      <c r="G14" s="5">
         <v>10038</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="H14" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I14" s="7">
+      <c r="I14" s="5">
         <v>4417</v>
       </c>
-      <c r="J14" s="7">
+      <c r="J14" s="5">
         <v>526</v>
       </c>
-      <c r="K14" s="7">
+      <c r="K14" s="5">
         <v>214</v>
       </c>
-      <c r="L14" s="7">
+      <c r="L14" s="5">
         <v>63023</v>
       </c>
-      <c r="M14" s="7">
+      <c r="M14" s="5">
         <v>5719</v>
       </c>
-      <c r="N14" s="7">
+      <c r="N14" s="5">
         <v>2445</v>
       </c>
-      <c r="O14" s="7">
+      <c r="O14" s="5">
         <v>4364</v>
       </c>
-      <c r="P14" s="7">
+      <c r="P14" s="5">
         <v>524</v>
       </c>
-      <c r="Q14" s="7">
+      <c r="Q14" s="5">
         <v>213</v>
       </c>
-      <c r="R14" s="7">
+      <c r="R14" s="5">
         <v>62996</v>
       </c>
-      <c r="S14" s="7">
+      <c r="S14" s="5">
         <v>5754</v>
       </c>
-      <c r="T14" s="8">
+      <c r="T14" s="6">
         <v>2443</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="10">
+      <c r="A15" s="15"/>
+      <c r="B15" s="7">
         <v>7772</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="7">
         <v>5464</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="7">
         <v>298</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="7">
         <v>97726</v>
       </c>
-      <c r="F15" s="10">
+      <c r="F15" s="7">
         <v>60252</v>
       </c>
-      <c r="G15" s="10">
+      <c r="G15" s="7">
         <v>3658</v>
       </c>
-      <c r="H15" s="10" t="s">
+      <c r="H15" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I15" s="10">
+      <c r="I15" s="7">
         <v>7829</v>
       </c>
-      <c r="J15" s="10">
+      <c r="J15" s="7">
         <v>320</v>
       </c>
-      <c r="K15" s="10">
+      <c r="K15" s="7">
         <v>89</v>
       </c>
-      <c r="L15" s="10">
+      <c r="L15" s="7">
         <v>76516</v>
       </c>
-      <c r="M15" s="10">
+      <c r="M15" s="7">
         <v>3777</v>
       </c>
-      <c r="N15" s="10">
+      <c r="N15" s="7">
         <v>894</v>
       </c>
-      <c r="O15" s="10">
+      <c r="O15" s="7">
         <v>7889</v>
       </c>
-      <c r="P15" s="10">
+      <c r="P15" s="7">
         <v>329</v>
       </c>
-      <c r="Q15" s="10">
+      <c r="Q15" s="7">
         <v>89</v>
       </c>
-      <c r="R15" s="10">
+      <c r="R15" s="7">
         <v>79627</v>
       </c>
-      <c r="S15" s="10">
+      <c r="S15" s="7">
         <v>3789</v>
       </c>
-      <c r="T15" s="11">
+      <c r="T15" s="8">
         <v>898</v>
       </c>
     </row>
-    <row r="17" spans="8:20" x14ac:dyDescent="0.25">
-      <c r="I17" s="2" t="s">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>4</v>
+      </c>
+      <c r="B19" s="2">
+        <v>154</v>
+      </c>
+      <c r="C19" s="2">
+        <v>513</v>
+      </c>
+      <c r="D19" s="2">
+        <v>307</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1702</v>
+      </c>
+      <c r="F19" s="2">
+        <v>5676</v>
+      </c>
+      <c r="G19" s="2">
+        <v>3476</v>
+      </c>
+      <c r="M19" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2" t="s">
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="12"/>
+      <c r="S19" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="P17" s="2"/>
-      <c r="Q17" s="2"/>
-      <c r="R17" s="2"/>
-      <c r="S17" s="2"/>
-      <c r="T17" s="2"/>
-    </row>
-    <row r="18" spans="8:20" x14ac:dyDescent="0.25">
-      <c r="H18" s="1" t="s">
+      <c r="T19" s="12"/>
+      <c r="U19" s="12"/>
+      <c r="V19" s="12"/>
+      <c r="W19" s="12"/>
+      <c r="X19" s="12"/>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B20" s="2">
+        <v>127</v>
+      </c>
+      <c r="C20" s="2">
+        <v>475</v>
+      </c>
+      <c r="D20" s="2">
+        <v>195</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1436</v>
+      </c>
+      <c r="F20" s="2">
+        <v>5451</v>
+      </c>
+      <c r="G20" s="2">
+        <v>2167</v>
+      </c>
+      <c r="L20" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="M20" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2" t="s">
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2" t="s">
+      <c r="Q20" s="12"/>
+      <c r="R20" s="12"/>
+      <c r="S20" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="2"/>
-      <c r="R18" s="2" t="s">
+      <c r="T20" s="12"/>
+      <c r="U20" s="12"/>
+      <c r="V20" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="S18" s="2"/>
-      <c r="T18" s="2"/>
-    </row>
-    <row r="19" spans="8:20" x14ac:dyDescent="0.25">
-      <c r="H19" s="1" t="s">
+      <c r="W20" s="12"/>
+      <c r="X20" s="12"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B21" s="2">
+        <v>153</v>
+      </c>
+      <c r="C21" s="2">
+        <v>727</v>
+      </c>
+      <c r="D21" s="1">
+        <v>85</v>
+      </c>
+      <c r="E21" s="2">
+        <v>1747</v>
+      </c>
+      <c r="F21" s="2">
+        <v>8935</v>
+      </c>
+      <c r="G21" s="2">
+        <v>854</v>
+      </c>
+      <c r="L21" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="M21" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="N21" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="O21" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L19" s="1" t="s">
+      <c r="P21" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="M19" s="1" t="s">
+      <c r="Q21" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="N19" s="1" t="s">
+      <c r="R21" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="O19" s="1" t="s">
+      <c r="S21" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P19" s="1" t="s">
+      <c r="T21" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="Q19" s="1" t="s">
+      <c r="U21" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="R19" s="1" t="s">
+      <c r="V21" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="S19" s="1" t="s">
+      <c r="W21" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="T19" s="1" t="s">
+      <c r="X21" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="8:20" x14ac:dyDescent="0.25">
-      <c r="H20" s="2">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>8</v>
+      </c>
+      <c r="B22" s="2">
+        <v>90</v>
+      </c>
+      <c r="C22" s="2">
+        <v>413</v>
+      </c>
+      <c r="D22" s="2">
+        <v>309</v>
+      </c>
+      <c r="E22" s="2">
+        <v>1011</v>
+      </c>
+      <c r="F22" s="2">
+        <v>4810</v>
+      </c>
+      <c r="G22" s="2">
+        <v>3485</v>
+      </c>
+      <c r="L22" s="12">
         <v>1024</v>
       </c>
-      <c r="I20" s="12">
+      <c r="M22" s="9">
         <v>30</v>
       </c>
-      <c r="J20" s="4">
+      <c r="N22" s="3">
         <v>208</v>
       </c>
-      <c r="K20" s="4">
+      <c r="O22" s="3">
         <v>365</v>
       </c>
-      <c r="L20" s="4">
+      <c r="P22" s="3">
         <v>360</v>
       </c>
-      <c r="M20" s="4">
+      <c r="Q22" s="3">
         <v>2467</v>
       </c>
-      <c r="N20" s="4">
+      <c r="R22" s="3">
         <v>4131</v>
       </c>
-      <c r="O20" s="4">
+      <c r="S22" s="3">
         <v>29</v>
       </c>
-      <c r="P20" s="4">
+      <c r="T22" s="3">
         <v>207</v>
       </c>
-      <c r="Q20" s="4">
+      <c r="U22" s="3">
         <v>358</v>
       </c>
-      <c r="R20" s="4">
+      <c r="V22" s="3">
         <v>358</v>
       </c>
-      <c r="S20" s="4">
+      <c r="W22" s="3">
         <v>2454</v>
       </c>
-      <c r="T20" s="5">
+      <c r="X22" s="4">
         <v>4121</v>
       </c>
     </row>
-    <row r="21" spans="8:20" x14ac:dyDescent="0.25">
-      <c r="H21" s="2"/>
-      <c r="I21" s="13">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B23" s="2">
+        <v>121</v>
+      </c>
+      <c r="C23" s="2">
+        <v>458</v>
+      </c>
+      <c r="D23" s="2">
+        <v>194</v>
+      </c>
+      <c r="E23" s="2">
+        <v>1337</v>
+      </c>
+      <c r="F23" s="2">
+        <v>5226</v>
+      </c>
+      <c r="G23" s="2">
+        <v>2155</v>
+      </c>
+      <c r="L23" s="12"/>
+      <c r="M23" s="10">
         <v>2948</v>
       </c>
-      <c r="J21" s="7">
+      <c r="N23" s="5">
         <v>416</v>
       </c>
-      <c r="K21" s="7">
+      <c r="O23" s="5">
         <v>211</v>
       </c>
-      <c r="L21" s="7">
+      <c r="P23" s="5">
         <v>30537</v>
       </c>
-      <c r="M21" s="7">
+      <c r="Q23" s="5">
         <v>4643</v>
       </c>
-      <c r="N21" s="7">
+      <c r="R23" s="5">
         <v>2382</v>
       </c>
-      <c r="O21" s="7">
+      <c r="S23" s="5">
         <v>2915</v>
       </c>
-      <c r="P21" s="7">
+      <c r="T23" s="5">
         <v>416</v>
       </c>
-      <c r="Q21" s="7">
+      <c r="U23" s="5">
         <v>212</v>
       </c>
-      <c r="R21" s="7">
+      <c r="V23" s="5">
         <v>30502</v>
       </c>
-      <c r="S21" s="7">
+      <c r="W23" s="5">
         <v>4660</v>
       </c>
-      <c r="T21" s="8">
+      <c r="X23" s="6">
         <v>2395</v>
       </c>
     </row>
-    <row r="22" spans="8:20" x14ac:dyDescent="0.25">
-      <c r="H22" s="2"/>
-      <c r="I22" s="13">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B24" s="2">
+        <v>123</v>
+      </c>
+      <c r="C24" s="2">
+        <v>546</v>
+      </c>
+      <c r="D24" s="2">
+        <v>84</v>
+      </c>
+      <c r="E24" s="2">
+        <v>1368</v>
+      </c>
+      <c r="F24" s="2">
+        <v>6471</v>
+      </c>
+      <c r="G24" s="2">
+        <v>844</v>
+      </c>
+      <c r="L24" s="12"/>
+      <c r="M24" s="10">
         <v>3924</v>
       </c>
-      <c r="J22" s="7">
+      <c r="N24" s="5">
         <v>241</v>
       </c>
-      <c r="K22" s="7">
+      <c r="O24" s="5">
         <v>88</v>
       </c>
-      <c r="L22" s="7">
+      <c r="P24" s="5">
         <v>39153</v>
       </c>
-      <c r="M22" s="7">
+      <c r="Q24" s="5">
         <v>3109</v>
       </c>
-      <c r="N22" s="7">
+      <c r="R24" s="5">
         <v>898</v>
       </c>
-      <c r="O22" s="7">
+      <c r="S24" s="5">
         <v>4086</v>
       </c>
-      <c r="P22" s="7">
+      <c r="T24" s="5">
         <v>240</v>
       </c>
-      <c r="Q22" s="7">
+      <c r="U24" s="5">
         <v>88</v>
       </c>
-      <c r="R22" s="7">
+      <c r="V24" s="5">
         <v>39046</v>
       </c>
-      <c r="S22" s="7">
+      <c r="W24" s="5">
         <v>3116</v>
       </c>
-      <c r="T22" s="8">
+      <c r="X24" s="6">
         <v>893</v>
       </c>
     </row>
-    <row r="23" spans="8:20" x14ac:dyDescent="0.25">
-      <c r="H23" s="2">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>16</v>
+      </c>
+      <c r="B25" s="2">
+        <v>66</v>
+      </c>
+      <c r="C25" s="2">
+        <v>384</v>
+      </c>
+      <c r="D25" s="2">
+        <v>308</v>
+      </c>
+      <c r="E25" s="2">
+        <v>719</v>
+      </c>
+      <c r="F25" s="2">
+        <v>4254</v>
+      </c>
+      <c r="G25" s="2">
+        <v>3478</v>
+      </c>
+      <c r="L25" s="12">
         <v>2048</v>
       </c>
-      <c r="I23" s="13">
+      <c r="M25" s="10">
         <v>30</v>
       </c>
-      <c r="J23" s="7">
+      <c r="N25" s="5">
         <v>211</v>
       </c>
-      <c r="K23" s="7">
+      <c r="O25" s="5">
         <v>362</v>
       </c>
-      <c r="L23" s="7">
+      <c r="P25" s="5">
         <v>312</v>
       </c>
-      <c r="M23" s="7">
+      <c r="Q25" s="5">
         <v>2426</v>
       </c>
-      <c r="N23" s="7">
+      <c r="R25" s="5">
         <v>4132</v>
       </c>
-      <c r="O23" s="7">
+      <c r="S25" s="5">
         <v>29</v>
       </c>
-      <c r="P23" s="7">
+      <c r="T25" s="5">
         <v>210</v>
       </c>
-      <c r="Q23" s="7">
+      <c r="U25" s="5">
         <v>359</v>
       </c>
-      <c r="R23" s="7">
+      <c r="V25" s="5">
         <v>306</v>
       </c>
-      <c r="S23" s="7">
+      <c r="W25" s="5">
         <v>2401</v>
       </c>
-      <c r="T23" s="8">
+      <c r="X25" s="6">
         <v>4112</v>
       </c>
     </row>
-    <row r="24" spans="8:20" x14ac:dyDescent="0.25">
-      <c r="H24" s="2"/>
-      <c r="I24" s="13">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B26" s="2">
+        <v>134</v>
+      </c>
+      <c r="C26" s="2">
+        <v>434</v>
+      </c>
+      <c r="D26" s="2">
+        <v>194</v>
+      </c>
+      <c r="E26" s="2">
+        <v>1479</v>
+      </c>
+      <c r="F26" s="2">
+        <v>4954</v>
+      </c>
+      <c r="G26" s="2">
+        <v>2164</v>
+      </c>
+      <c r="L26" s="12"/>
+      <c r="M26" s="10">
         <v>4423</v>
       </c>
-      <c r="J24" s="7">
+      <c r="N26" s="5">
         <v>427</v>
       </c>
-      <c r="K24" s="7">
+      <c r="O26" s="5">
         <v>211</v>
       </c>
-      <c r="L24" s="7">
+      <c r="P26" s="5">
         <v>63151</v>
       </c>
-      <c r="M24" s="7">
+      <c r="Q26" s="5">
         <v>4710</v>
       </c>
-      <c r="N24" s="7">
+      <c r="R26" s="5">
         <v>2399</v>
       </c>
-      <c r="O24" s="7">
+      <c r="S26" s="5">
         <v>4418</v>
       </c>
-      <c r="P24" s="7">
+      <c r="T26" s="5">
         <v>427</v>
       </c>
-      <c r="Q24" s="7">
+      <c r="U26" s="5">
         <v>211</v>
       </c>
-      <c r="R24" s="7">
+      <c r="V26" s="5">
         <v>63094</v>
       </c>
-      <c r="S24" s="7">
+      <c r="W26" s="5">
         <v>4700</v>
       </c>
-      <c r="T24" s="8">
+      <c r="X26" s="6">
         <v>2399</v>
       </c>
     </row>
-    <row r="25" spans="8:20" x14ac:dyDescent="0.25">
-      <c r="H25" s="2"/>
-      <c r="I25" s="14">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B27" s="2">
+        <v>133</v>
+      </c>
+      <c r="C27" s="2">
+        <v>470</v>
+      </c>
+      <c r="D27" s="2">
+        <v>85</v>
+      </c>
+      <c r="E27" s="2">
+        <v>1463</v>
+      </c>
+      <c r="F27" s="2">
+        <v>5417</v>
+      </c>
+      <c r="G27" s="2">
+        <v>846</v>
+      </c>
+      <c r="L27" s="12"/>
+      <c r="M27" s="11">
         <v>7955</v>
       </c>
-      <c r="J25" s="10">
+      <c r="N27" s="7">
         <v>250</v>
       </c>
-      <c r="K25" s="10">
+      <c r="O27" s="7">
         <v>88</v>
       </c>
-      <c r="L25" s="10">
+      <c r="P27" s="7">
         <v>79485</v>
       </c>
-      <c r="M25" s="10">
+      <c r="Q27" s="7">
         <v>3601</v>
       </c>
-      <c r="N25" s="10">
+      <c r="R27" s="7">
         <v>1156</v>
       </c>
-      <c r="O25" s="10">
+      <c r="S27" s="7">
         <v>7849</v>
       </c>
-      <c r="P25" s="10">
+      <c r="T27" s="7">
         <v>246</v>
       </c>
-      <c r="Q25" s="10">
+      <c r="U27" s="7">
         <v>88</v>
       </c>
-      <c r="R25" s="10">
+      <c r="V27" s="7">
         <v>78337</v>
       </c>
-      <c r="S25" s="10">
+      <c r="W27" s="7">
         <v>2838</v>
       </c>
-      <c r="T25" s="11">
+      <c r="X27" s="8">
         <v>894</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="O17:T17"/>
-    <mergeCell ref="I17:N17"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="L18:N18"/>
-    <mergeCell ref="H23:H25"/>
-    <mergeCell ref="H20:H22"/>
-    <mergeCell ref="O18:Q18"/>
-    <mergeCell ref="R18:T18"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A13:A15"/>
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="I1:N1"/>
     <mergeCell ref="I2:K2"/>
@@ -1734,10 +1907,14 @@
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="E2:G2"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="S19:X19"/>
+    <mergeCell ref="M19:R19"/>
+    <mergeCell ref="M20:O20"/>
+    <mergeCell ref="P20:R20"/>
+    <mergeCell ref="L25:L27"/>
+    <mergeCell ref="L22:L24"/>
+    <mergeCell ref="S20:U20"/>
+    <mergeCell ref="V20:X20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>